<commit_message>
Checked and Answerd the CYRS Review and modified the CYRS to proposed V1.3 Signed-off-by: MostafaNader96 <mnader96@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS_Review.xlsx
+++ b/Input documents/CYRS_Review.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -171,11 +171,32 @@
   <si>
     <t xml:space="preserve">All Req need to be updated with system level prospective not SW prospective </t>
   </si>
+  <si>
+    <t>This is already included in the document history</t>
+  </si>
+  <si>
+    <t>Modified</t>
+  </si>
+  <si>
+    <t>Modified, and document history is moved to the start of the document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As the HSI is the document related to the chosen HW components so in the CYRS for example a displayer in the high level and in the HSI its specified to a 16*2 lcd </t>
+  </si>
+  <si>
+    <t>Modified as a system and not software requirements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiss requirement describes a high level relation between the HW component""Buzzer"  that will be referenced to the HIS and a SW requirement"That buzzer is on when specific time is hit" that will be referenced to the SRS </t>
+  </si>
+  <si>
+    <t>The reference table that references each requirement to its parent requirement in the CRS document is at the end of the CYRS document</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -540,12 +561,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -557,36 +608,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -935,199 +956,216 @@
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="D9" sqref="D9:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25" t="s">
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="28"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="29"/>
-    </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="26"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="29"/>
-    </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="24" t="s">
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="38"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="39"/>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="39"/>
+    </row>
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="30" t="s">
+      <c r="C6" s="32"/>
+      <c r="D6" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="31"/>
-    </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="24" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="30" t="s">
+      <c r="C7" s="32"/>
+      <c r="D7" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="24" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="25"/>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="30" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
+      <c r="H8" s="25"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="30" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="32" t="s">
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="30"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33" t="s">
+      <c r="D12" s="34"/>
+      <c r="E12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="34"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="35"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30" t="s">
+      <c r="D13" s="24"/>
+      <c r="E13" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30" t="s">
+      <c r="F13" s="24"/>
+      <c r="G13" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="31"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H13" s="25"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="31"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="25"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="25"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="36"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1144,23 +1182,6 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1171,24 +1192,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" customWidth="1"/>
+    <col min="12" max="12" width="174.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1217,7 +1238,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
@@ -1236,13 +1257,17 @@
       <c r="F2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="10"/>
-    </row>
-    <row r="3" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="I2" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>36</v>
       </c>
@@ -1261,16 +1286,20 @@
       <c r="F3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="10"/>
+      <c r="I3" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="K3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>36</v>
       </c>
@@ -1289,16 +1318,20 @@
       <c r="F4" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="K4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
@@ -1317,13 +1350,17 @@
       <c r="F5" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="12"/>
-    </row>
-    <row r="6" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="I5" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -1342,16 +1379,20 @@
       <c r="F6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="H6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="12"/>
+      <c r="I6" s="12" t="s">
+        <v>50</v>
+      </c>
       <c r="K6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
@@ -1370,16 +1411,20 @@
       <c r="F7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="H7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="12"/>
+      <c r="I7" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="K7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>36</v>
       </c>
@@ -1398,13 +1443,17 @@
       <c r="F8" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="10"/>
+      <c r="G8" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I8" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="13"/>
@@ -1415,7 +1464,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="13"/>
@@ -1432,7 +1481,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="13"/>
@@ -1449,7 +1498,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="13"/>
@@ -1460,7 +1509,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="13"/>
@@ -1471,7 +1520,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="13"/>
@@ -1482,7 +1531,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1493,7 +1542,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -1504,7 +1553,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -1515,7 +1564,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -1526,7 +1575,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
@@ -1537,7 +1586,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -1548,7 +1597,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1559,7 +1608,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -1570,7 +1619,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
@@ -1581,7 +1630,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
@@ -1592,7 +1641,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
@@ -1603,7 +1652,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1614,7 +1663,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -1625,7 +1674,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1636,7 +1685,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1647,7 +1696,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1658,7 +1707,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1669,7 +1718,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1680,7 +1729,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -1691,7 +1740,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -1702,7 +1751,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1713,7 +1762,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1724,7 +1773,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1735,7 +1784,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1746,7 +1795,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1757,7 +1806,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1768,7 +1817,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1779,7 +1828,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1790,7 +1839,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1801,7 +1850,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1812,7 +1861,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -1823,7 +1872,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>

</xml_diff>

<commit_message>
Update Review sheets CYRS , and HSI
</commit_message>
<xml_diff>
--- a/Input documents/CYRS_Review.xlsx
+++ b/Input documents/CYRS_Review.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t xml:space="preserve">V1.2 </t>
-  </si>
-  <si>
-    <t>V1.2</t>
   </si>
   <si>
     <t xml:space="preserve">Document History </t>
@@ -192,11 +189,24 @@
   <si>
     <t>The reference table that references each requirement to its parent requirement in the CRS document is at the end of the CYRS document</t>
   </si>
+  <si>
+    <t>V1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update the status for each req </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is lots of use cases are not mentioned in terms of system req Like :
+- How to navigate between modes 
+- what are the functions of each button in each mode 
+- how to adjust the time and minute for each mode 
+- etc </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -496,7 +506,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -561,12 +571,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -582,32 +619,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -956,216 +969,207 @@
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:H9"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="32.28515625" customWidth="1"/>
+    <col min="8" max="8" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="31" t="s">
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32" t="s">
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="38"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="39"/>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="39"/>
-    </row>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="31" t="s">
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="28"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="24" t="s">
+      <c r="C6" s="25"/>
+      <c r="D6" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="31" t="s">
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+    </row>
+    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25"/>
-    </row>
-    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="31" t="s">
+      <c r="C7" s="25"/>
+      <c r="D7" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
+    </row>
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="24" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="25"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="25"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="30"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="33" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="40">
+        <v>44076</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="39"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="35"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="34"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34" t="s">
+      <c r="D12" s="33"/>
+      <c r="E12" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34" t="s">
+      <c r="F12" s="33"/>
+      <c r="G12" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="35"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="34"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24" t="s">
+      <c r="D13" s="30"/>
+      <c r="E13" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24" t="s">
+      <c r="F13" s="30"/>
+      <c r="G13" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="H13" s="25"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="25"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="31"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="30"/>
+      <c r="E14" s="40">
+        <v>44076</v>
+      </c>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" s="31"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="25"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="25"/>
-    </row>
-    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="27"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B3:D5"/>
-    <mergeCell ref="E3:H5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:H8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -1182,6 +1186,23 @@
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="G14:H14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:H8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="B3:D5"/>
+    <mergeCell ref="E3:H5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -1192,24 +1213,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="39.85546875" customWidth="1"/>
-    <col min="12" max="12" width="174.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.88671875" customWidth="1"/>
+    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1238,7 +1259,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
@@ -1261,13 +1282,13 @@
         <v>20</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>36</v>
       </c>
@@ -1281,25 +1302,25 @@
         <v>31</v>
       </c>
       <c r="E3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>39</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>20</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>36</v>
       </c>
@@ -1316,22 +1337,22 @@
         <v>34</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
@@ -1345,22 +1366,22 @@
         <v>31</v>
       </c>
       <c r="E5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -1377,22 +1398,22 @@
         <v>34</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>21</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
@@ -1409,22 +1430,22 @@
         <v>34</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>36</v>
       </c>
@@ -1441,30 +1462,44 @@
         <v>34</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="H8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>44076</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
       <c r="I9" s="12"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="13"/>
@@ -1481,7 +1516,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="13"/>
@@ -1498,7 +1533,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="13"/>
@@ -1509,7 +1544,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="13"/>
@@ -1520,7 +1555,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="13"/>
@@ -1531,7 +1566,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1542,7 +1577,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -1553,7 +1588,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -1564,7 +1599,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -1575,7 +1610,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
@@ -1586,7 +1621,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -1597,7 +1632,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1608,7 +1643,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -1619,7 +1654,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
@@ -1630,7 +1665,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
@@ -1641,7 +1676,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
@@ -1652,7 +1687,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1663,7 +1698,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -1674,7 +1709,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1685,7 +1720,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1696,7 +1731,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1707,7 +1742,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1718,7 +1753,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1729,7 +1764,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -1740,7 +1775,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -1751,7 +1786,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1762,7 +1797,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1773,7 +1808,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1784,7 +1819,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1795,7 +1830,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1806,7 +1841,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1817,7 +1852,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1828,7 +1863,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1839,7 +1874,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1850,7 +1885,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1861,7 +1896,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -1872,7 +1907,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>

</xml_diff>

<commit_message>
Added version 1.6 of the CYRS including 4 new requirements and modified the CYRS_Review sheet Signed-off-by: MostafaNader96 <mnader96@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/CYRS_Review.xlsx
+++ b/Input documents/CYRS_Review.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -169,9 +169,6 @@
     <t xml:space="preserve">All Req need to be updated with system level prospective not SW prospective </t>
   </si>
   <si>
-    <t>This is already included in the document history</t>
-  </si>
-  <si>
     <t>Modified</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
   </si>
   <si>
     <t xml:space="preserve">Thiss requirement describes a high level relation between the HW component""Buzzer"  that will be referenced to the HIS and a SW requirement"That buzzer is on when specific time is hit" that will be referenced to the SRS </t>
-  </si>
-  <si>
-    <t>The reference table that references each requirement to its parent requirement in the CRS document is at the end of the CYRS document</t>
   </si>
   <si>
     <t>V1.5</t>
@@ -202,11 +196,20 @@
 - how to adjust the time and minute for each mode 
 - etc </t>
   </si>
+  <si>
+    <t>Added Document status table</t>
+  </si>
+  <si>
+    <t>Added reference table at the end of the document</t>
+  </si>
+  <si>
+    <t>Added the needed requirements</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -595,6 +598,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -617,9 +623,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -972,13 +975,13 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
@@ -991,7 +994,7 @@
       <c r="G3" s="25"/>
       <c r="H3" s="28"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="26"/>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
@@ -1000,7 +1003,7 @@
       <c r="G4" s="27"/>
       <c r="H4" s="29"/>
     </row>
-    <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="26"/>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
@@ -1009,7 +1012,7 @@
       <c r="G5" s="27"/>
       <c r="H5" s="29"/>
     </row>
-    <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
         <v>1</v>
       </c>
@@ -1022,20 +1025,20 @@
       <c r="G6" s="30"/>
       <c r="H6" s="31"/>
     </row>
-    <row r="7" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="24" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
       <c r="H7" s="31"/>
     </row>
-    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
         <v>3</v>
       </c>
@@ -1048,12 +1051,12 @@
       <c r="G8" s="30"/>
       <c r="H8" s="31"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="25"/>
-      <c r="D9" s="40">
+      <c r="D9" s="32">
         <v>44076</v>
       </c>
       <c r="E9" s="30"/>
@@ -1061,44 +1064,44 @@
       <c r="G9" s="30"/>
       <c r="H9" s="31"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="32" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="40"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="34"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="35"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33" t="s">
+      <c r="D12" s="34"/>
+      <c r="E12" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="34"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="35"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>0.1</v>
       </c>
@@ -1115,7 +1118,7 @@
       </c>
       <c r="H13" s="31"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>0.2</v>
       </c>
@@ -1123,16 +1126,16 @@
         <v>29</v>
       </c>
       <c r="D14" s="30"/>
-      <c r="E14" s="40">
+      <c r="E14" s="32">
         <v>44076</v>
       </c>
       <c r="F14" s="30"/>
       <c r="G14" s="30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H14" s="31"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
@@ -1141,7 +1144,7 @@
       <c r="G15" s="30"/>
       <c r="H15" s="31"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
@@ -1150,7 +1153,7 @@
       <c r="G16" s="30"/>
       <c r="H16" s="31"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
@@ -1159,14 +1162,14 @@
       <c r="G17" s="30"/>
       <c r="H17" s="31"/>
     </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="33">
@@ -1213,24 +1216,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="100.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="100.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="39.88671875" customWidth="1"/>
-    <col min="12" max="12" width="174.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" customWidth="1"/>
+    <col min="12" max="12" width="174.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -1259,7 +1262,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
@@ -1285,10 +1288,10 @@
         <v>22</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>36</v>
       </c>
@@ -1314,13 +1317,13 @@
         <v>22</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>36</v>
       </c>
@@ -1346,13 +1349,13 @@
         <v>22</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
@@ -1378,10 +1381,10 @@
         <v>22</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -1401,19 +1404,19 @@
         <v>43</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>22</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>36</v>
       </c>
@@ -1433,19 +1436,19 @@
         <v>44</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>22</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>36</v>
       </c>
@@ -1471,10 +1474,10 @@
         <v>22</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>44076</v>
       </c>
@@ -1482,7 +1485,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>31</v>
@@ -1491,15 +1494,19 @@
         <v>34</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="10"/>
+        <v>53</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>20</v>
+      </c>
       <c r="H9" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="I9" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="13"/>
@@ -1516,7 +1523,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="13"/>
@@ -1533,7 +1540,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="13"/>
@@ -1544,7 +1551,7 @@
       <c r="H12" s="10"/>
       <c r="I12" s="12"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="13"/>
@@ -1555,7 +1562,7 @@
       <c r="H13" s="10"/>
       <c r="I13" s="12"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="13"/>
@@ -1566,7 +1573,7 @@
       <c r="H14" s="10"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1577,7 +1584,7 @@
       <c r="H15" s="10"/>
       <c r="I15" s="19"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
@@ -1588,7 +1595,7 @@
       <c r="H16" s="10"/>
       <c r="I16" s="19"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="15"/>
       <c r="C17" s="16"/>
@@ -1599,7 +1606,7 @@
       <c r="H17" s="10"/>
       <c r="I17" s="19"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="16"/>
@@ -1610,7 +1617,7 @@
       <c r="H18" s="10"/>
       <c r="I18" s="19"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="16"/>
@@ -1621,7 +1628,7 @@
       <c r="H19" s="10"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
@@ -1632,7 +1639,7 @@
       <c r="H20" s="10"/>
       <c r="I20" s="19"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="16"/>
@@ -1643,7 +1650,7 @@
       <c r="H21" s="10"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="16"/>
@@ -1654,7 +1661,7 @@
       <c r="H22" s="10"/>
       <c r="I22" s="19"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="15"/>
       <c r="C23" s="16"/>
@@ -1665,7 +1672,7 @@
       <c r="H23" s="10"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="16"/>
@@ -1676,7 +1683,7 @@
       <c r="H24" s="10"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
@@ -1687,7 +1694,7 @@
       <c r="H25" s="10"/>
       <c r="I25" s="19"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="15"/>
       <c r="C26" s="16"/>
@@ -1698,7 +1705,7 @@
       <c r="H26" s="10"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -1709,7 +1716,7 @@
       <c r="H27" s="10"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1720,7 +1727,7 @@
       <c r="H28" s="10"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1731,7 +1738,7 @@
       <c r="H29" s="10"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1742,7 +1749,7 @@
       <c r="H30" s="10"/>
       <c r="I30" s="19"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="16"/>
@@ -1753,7 +1760,7 @@
       <c r="H31" s="10"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -1764,7 +1771,7 @@
       <c r="H32" s="10"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
@@ -1775,7 +1782,7 @@
       <c r="H33" s="10"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -1786,7 +1793,7 @@
       <c r="H34" s="10"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -1797,7 +1804,7 @@
       <c r="H35" s="10"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -1808,7 +1815,7 @@
       <c r="H36" s="10"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -1819,7 +1826,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="19"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -1830,7 +1837,7 @@
       <c r="H38" s="10"/>
       <c r="I38" s="19"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -1841,7 +1848,7 @@
       <c r="H39" s="10"/>
       <c r="I39" s="19"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -1852,7 +1859,7 @@
       <c r="H40" s="10"/>
       <c r="I40" s="19"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -1863,7 +1870,7 @@
       <c r="H41" s="10"/>
       <c r="I41" s="19"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -1874,7 +1881,7 @@
       <c r="H42" s="10"/>
       <c r="I42" s="19"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -1885,7 +1892,7 @@
       <c r="H43" s="10"/>
       <c r="I43" s="19"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="16"/>
@@ -1896,7 +1903,7 @@
       <c r="H44" s="10"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="16"/>
@@ -1907,7 +1914,7 @@
       <c r="H45" s="10"/>
       <c r="I45" s="19"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>

</xml_diff>

<commit_message>
Update review sheets for CYRS and HSI
</commit_message>
<xml_diff>
--- a/Input documents/CYRS_Review.xlsx
+++ b/Input documents/CYRS_Review.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction " sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
   <si>
     <t xml:space="preserve">Project Name </t>
   </si>
@@ -203,13 +203,26 @@
     <t>Added reference table at the end of the document</t>
   </si>
   <si>
-    <t>Added the needed requirements</t>
+    <t>Added the needed requirements
+TSH: I mean here the system doesn't descrip those use cases , are you able to handle all these use cases in the SRS req , if yes then it is ok for me ?</t>
+  </si>
+  <si>
+    <t>14/2/202</t>
+  </si>
+  <si>
+    <t>Update the status of the last open point</t>
+  </si>
+  <si>
+    <t>V1.6</t>
+  </si>
+  <si>
+    <t>14/2/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -971,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,7 +1044,7 @@
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="30" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
@@ -1056,8 +1069,8 @@
         <v>9</v>
       </c>
       <c r="C9" s="25"/>
-      <c r="D9" s="32">
-        <v>44076</v>
+      <c r="D9" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="30"/>
@@ -1136,12 +1149,20 @@
       <c r="H14" s="31"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
-      <c r="C15" s="30"/>
+      <c r="B15" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>29</v>
+      </c>
       <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
+      <c r="E15" s="30" t="s">
+        <v>57</v>
+      </c>
       <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
+      <c r="G15" s="30" t="s">
+        <v>58</v>
+      </c>
       <c r="H15" s="31"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -1216,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,9 +1521,9 @@
         <v>20</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="10" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>